<commit_message>
version 5,09,24 excel table
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,112 +440,405 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>Дата создания</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Проблема</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>User ID</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ИМЯ/First Name</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ФАМИЛИЯ/Last Name</t>
+          <t>ИМЯ</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>ЛОГИН/Username</t>
+          <t>ФАМИЛИЯ</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>question1</t>
+          <t>ЛОГИН</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>question2</t>
+          <t>Ответ1</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>question3</t>
+          <t>Ответ2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Ответ3</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Почта</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Доп.вопрос</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" s="2" t="n">
+        <v>45539.90326388889</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Куда вводить код</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>6625770047</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>kiper_slivki</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45539.9024074074</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Не пришел код</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>1006569664</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Roman</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Chiper</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>RomanKiper</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Первый вопросительный</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Пололрппппппвапррррррррр</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Лллллллллллппппееннннеепееееенепппппееее</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>@ ккккк</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45539.89626157407</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Помощь с подбором курса</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>6625770047</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>kiper_slivki</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Всякую</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>По всякому</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Всякийлллллллллооо</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Пророоо</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ллллллллллллллллллллллллоьттиииииииииииииииииииииииииииииииииииииииииииииммммммммммми</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Рррроооооол</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45539.89578703704</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Нет моего вопроса</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>6625770047</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>kiper_slivki</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Срочный вопрос оооооооооо́лльььььььььььььььььььььььььььььььььььььооооорррррррррпааапроолллооооооооооооотторррииииррррррппппммирррооллььььььььььььььь</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45539.89491898148</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Не пришел код</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>6625770047</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>kiper_slivki</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Почта@руу</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45539.88535879629</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Нет моего вопроса</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1006569664</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Roman</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Chiper</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>RomanKiper</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Привет админ
+Моего вопроса нет в списке
+Что делать
+У меня вопрос следущий
+Я переживаю чтотеет моего вопросаротьььььбббьлооооррроооориррррролллллдддддддд</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45539.8768287037</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Не могу войти в аккаунт</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1006569664</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Roman</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Chiper</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>RomanKiper</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Дуда@mail</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45539.87126157407</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Не работает код</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1006569664</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Roman</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Chiper</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>RomanKiper</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45539.86407407407</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Куда вводить код</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1006569664</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Roman</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Chiper</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>RomanKiper</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45539.85804398148</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Помощь с подбором курса</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1006569664</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Roman</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Chiper</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>RomanKiper</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>одинннн</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>дваааа</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>трииии</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>